<commit_message>
intermediate state - moving to google ruby api_client
</commit_message>
<xml_diff>
--- a/calendar-base.xlsx
+++ b/calendar-base.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="calendar-base.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'calendar-base.csv'!$H$1:$H$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'calendar-base.csv'!$G$1:$H$106</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="119">
   <si>
     <t>Month</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Session</t>
   </si>
   <si>
-    <t>Aug</t>
-  </si>
-  <si>
     <t>9:00AM till 10:30AM</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
   </si>
   <si>
     <t>Common Group Coaching Session</t>
-  </si>
-  <si>
-    <t>Sep</t>
   </si>
   <si>
     <t>Welcome to TWU</t>
@@ -1006,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1022,7 +1016,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>0</v>
@@ -1037,33 +1031,29 @@
         <v>3</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H1" s="41" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="21">
-        <v>30</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
       <c r="D2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="21" t="s">
-        <v>6</v>
-      </c>
       <c r="F2" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>3</v>
@@ -1074,17 +1064,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="22"/>
-      <c r="B3" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="22">
-        <v>30</v>
-      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>8</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="3" t="s">
@@ -1096,17 +1082,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="22"/>
-      <c r="B4" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="22">
-        <v>30</v>
-      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>10</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="3" t="s">
@@ -1118,17 +1100,13 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="22"/>
-      <c r="B5" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="22">
-        <v>30</v>
-      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>11</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>12</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="3" t="s">
@@ -1140,17 +1118,13 @@
     </row>
     <row r="6" spans="1:8" ht="16" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="23">
-        <v>30</v>
-      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>14</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="4" t="s">
@@ -1162,19 +1136,15 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="24">
-        <v>2</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="5" t="s">
@@ -1186,17 +1156,13 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="25"/>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="25" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="25">
-        <v>2</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>17</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="6" t="s">
@@ -1208,17 +1174,13 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="25"/>
-      <c r="B9" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="25">
-        <v>2</v>
-      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="6" t="s">
@@ -1230,17 +1192,13 @@
     </row>
     <row r="10" spans="1:8" ht="16" thickBot="1">
       <c r="A10" s="26"/>
-      <c r="B10" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="26">
-        <v>2</v>
-      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="7" t="s">
@@ -1252,19 +1210,15 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="24">
-        <v>3</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F11" s="24"/>
       <c r="G11" s="5" t="s">
@@ -1276,17 +1230,13 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="25"/>
-      <c r="B12" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="25">
-        <v>3</v>
-      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="6" t="s">
@@ -1298,17 +1248,13 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="25"/>
-      <c r="B13" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="25">
-        <v>3</v>
-      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="6" t="s">
@@ -1320,17 +1266,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="25"/>
-      <c r="B14" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="25">
-        <v>3</v>
-      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="6" t="s">
@@ -1342,21 +1284,17 @@
     </row>
     <row r="15" spans="1:8" ht="16" thickBot="1">
       <c r="A15" s="26"/>
-      <c r="B15" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="26">
-        <v>3</v>
-      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F15" s="26"/>
       <c r="G15" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H15" s="25">
         <v>1</v>
@@ -1364,19 +1302,15 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="25">
-        <v>4</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="27" t="s">
@@ -1388,17 +1322,13 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="25"/>
-      <c r="B17" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="25">
-        <v>4</v>
-      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F17" s="25"/>
       <c r="G17" s="27" t="s">
@@ -1410,21 +1340,17 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="25"/>
-      <c r="B18" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="25">
-        <v>4</v>
-      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
       <c r="D18" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H18" s="25">
         <v>1</v>
@@ -1432,21 +1358,17 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="25"/>
-      <c r="B19" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="25">
-        <v>4</v>
-      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
       <c r="D19" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H19" s="25">
         <v>1</v>
@@ -1454,21 +1376,17 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="25"/>
-      <c r="B20" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="25">
-        <v>4</v>
-      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F20" s="25"/>
       <c r="G20" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H20" s="25">
         <v>1</v>
@@ -1476,17 +1394,13 @@
     </row>
     <row r="21" spans="1:8" ht="16" thickBot="1">
       <c r="A21" s="26"/>
-      <c r="B21" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="26">
-        <v>4</v>
-      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F21" s="26"/>
       <c r="G21" s="7" t="s">
@@ -1498,19 +1412,15 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="24">
-        <v>5</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F22" s="24"/>
       <c r="G22" s="5" t="s">
@@ -1522,21 +1432,17 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="25"/>
-      <c r="B23" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="25">
-        <v>5</v>
-      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H23" s="25">
         <v>1</v>
@@ -1544,21 +1450,17 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="25"/>
-      <c r="B24" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="25">
-        <v>5</v>
-      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F24" s="25"/>
       <c r="G24" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H24" s="25">
         <v>1</v>
@@ -1566,21 +1468,17 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="25"/>
-      <c r="B25" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="25">
-        <v>5</v>
-      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H25" s="25">
         <v>1</v>
@@ -1588,21 +1486,17 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="25"/>
-      <c r="B26" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="25">
-        <v>5</v>
-      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F26" s="25"/>
       <c r="G26" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H26" s="25">
         <v>1</v>
@@ -1610,21 +1504,17 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="25"/>
-      <c r="B27" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="25">
-        <v>5</v>
-      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F27" s="25"/>
       <c r="G27" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H27" s="25">
         <v>1</v>
@@ -1632,21 +1522,17 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="25"/>
-      <c r="B28" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="25">
-        <v>5</v>
-      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F28" s="25"/>
       <c r="G28" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H28" s="25">
         <v>1</v>
@@ -1654,21 +1540,17 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="25"/>
-      <c r="B29" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="25">
-        <v>5</v>
-      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F29" s="25"/>
       <c r="G29" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H29" s="25">
         <v>1</v>
@@ -1676,21 +1558,17 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="25"/>
-      <c r="B30" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="25">
-        <v>5</v>
-      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F30" s="25"/>
       <c r="G30" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H30" s="25">
         <v>1</v>
@@ -1698,21 +1576,17 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="25"/>
-      <c r="B31" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="25">
-        <v>5</v>
-      </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F31" s="25"/>
       <c r="G31" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H31" s="25">
         <v>1</v>
@@ -1720,21 +1594,17 @@
     </row>
     <row r="32" spans="1:8" ht="16" thickBot="1">
       <c r="A32" s="26"/>
-      <c r="B32" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="26">
-        <v>5</v>
-      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F32" s="26"/>
       <c r="G32" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H32" s="25">
         <v>1</v>
@@ -1742,19 +1612,15 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="24">
-        <v>6</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
       <c r="D33" s="24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="5" t="s">
@@ -1766,21 +1632,17 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="25"/>
-      <c r="B34" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="25">
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="25" t="s">
-        <v>7</v>
-      </c>
       <c r="E34" s="25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F34" s="25"/>
       <c r="G34" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H34" s="25">
         <v>1</v>
@@ -1788,21 +1650,17 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="25"/>
-      <c r="B35" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="25">
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="25" t="s">
-        <v>7</v>
-      </c>
       <c r="E35" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F35" s="25"/>
       <c r="G35" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H35" s="25">
         <v>1</v>
@@ -1810,21 +1668,17 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="25"/>
-      <c r="B36" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="25">
-        <v>6</v>
-      </c>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
       <c r="D36" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H36" s="25">
         <v>1</v>
@@ -1832,21 +1686,17 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="25"/>
-      <c r="B37" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="25">
-        <v>6</v>
-      </c>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F37" s="25"/>
       <c r="G37" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H37" s="25">
         <v>1</v>
@@ -1854,21 +1704,17 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="25"/>
-      <c r="B38" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="25">
-        <v>6</v>
-      </c>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F38" s="25"/>
       <c r="G38" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H38" s="25">
         <v>1</v>
@@ -1876,21 +1722,17 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="25"/>
-      <c r="B39" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="25">
-        <v>6</v>
-      </c>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
       <c r="D39" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H39" s="25">
         <v>1</v>
@@ -1898,21 +1740,17 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="25"/>
-      <c r="B40" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="25">
-        <v>6</v>
-      </c>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
       <c r="D40" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E40" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F40" s="25"/>
       <c r="G40" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H40" s="25">
         <v>1</v>
@@ -1920,21 +1758,17 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="25"/>
-      <c r="B41" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="25">
-        <v>6</v>
-      </c>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
       <c r="D41" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F41" s="25"/>
       <c r="G41" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H41" s="25">
         <v>1</v>
@@ -1942,21 +1776,17 @@
     </row>
     <row r="42" spans="1:8" ht="16" thickBot="1">
       <c r="A42" s="26"/>
-      <c r="B42" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="26">
-        <v>6</v>
-      </c>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
       <c r="D42" s="26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F42" s="26"/>
       <c r="G42" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H42" s="26">
         <v>1</v>
@@ -1964,19 +1794,15 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="B43" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="28">
-        <v>9</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
       <c r="D43" s="28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F43" s="28"/>
       <c r="G43" s="8" t="s">
@@ -1988,21 +1814,17 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="29"/>
-      <c r="B44" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="29">
-        <v>9</v>
-      </c>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
       <c r="D44" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F44" s="29"/>
       <c r="G44" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H44" s="29">
         <v>2</v>
@@ -2010,21 +1832,17 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="29"/>
-      <c r="B45" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C45" s="29">
-        <v>9</v>
-      </c>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
       <c r="D45" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F45" s="29"/>
       <c r="G45" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H45" s="29">
         <v>2</v>
@@ -2032,17 +1850,13 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="29"/>
-      <c r="B46" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" s="29">
-        <v>9</v>
-      </c>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
       <c r="D46" s="29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F46" s="29"/>
       <c r="G46" s="9" t="s">
@@ -2054,21 +1868,17 @@
     </row>
     <row r="47" spans="1:8" ht="16" thickBot="1">
       <c r="A47" s="30"/>
-      <c r="B47" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C47" s="30">
-        <v>9</v>
-      </c>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
       <c r="D47" s="30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E47" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F47" s="30"/>
       <c r="G47" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H47" s="29">
         <v>2</v>
@@ -2076,23 +1886,19 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="B48" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="28">
-        <v>10</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
       <c r="D48" s="28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F48" s="28"/>
       <c r="G48" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H48" s="29">
         <v>2</v>
@@ -2100,21 +1906,17 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="29"/>
-      <c r="B49" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="29">
-        <v>10</v>
-      </c>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
       <c r="D49" s="29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F49" s="29"/>
       <c r="G49" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H49" s="29">
         <v>2</v>
@@ -2122,21 +1924,17 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="29"/>
-      <c r="B50" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" s="29">
-        <v>10</v>
-      </c>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
       <c r="D50" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F50" s="29"/>
       <c r="G50" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H50" s="29">
         <v>2</v>
@@ -2144,21 +1942,17 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="29"/>
-      <c r="B51" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C51" s="29">
-        <v>10</v>
-      </c>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
       <c r="D51" s="29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F51" s="29"/>
       <c r="G51" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H51" s="29">
         <v>2</v>
@@ -2166,21 +1960,17 @@
     </row>
     <row r="52" spans="1:8" ht="16" thickBot="1">
       <c r="A52" s="30"/>
-      <c r="B52" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C52" s="30">
-        <v>10</v>
-      </c>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
       <c r="D52" s="30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E52" s="30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F52" s="30"/>
       <c r="G52" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H52" s="29">
         <v>2</v>
@@ -2188,19 +1978,15 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="B53" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" s="28">
-        <v>11</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
       <c r="D53" s="28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F53" s="28"/>
       <c r="G53" s="8" t="s">
@@ -2212,21 +1998,17 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="29"/>
-      <c r="B54" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" s="29">
-        <v>11</v>
-      </c>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
       <c r="D54" s="29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F54" s="29"/>
       <c r="G54" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H54" s="29">
         <v>2</v>
@@ -2234,21 +2016,17 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="29"/>
-      <c r="B55" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" s="29">
-        <v>11</v>
-      </c>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
       <c r="D55" s="29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F55" s="29"/>
       <c r="G55" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H55" s="29">
         <v>2</v>
@@ -2256,21 +2034,17 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="29"/>
-      <c r="B56" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" s="29">
-        <v>11</v>
-      </c>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
       <c r="D56" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F56" s="29"/>
       <c r="G56" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H56" s="29">
         <v>2</v>
@@ -2278,21 +2052,17 @@
     </row>
     <row r="57" spans="1:8" ht="16" thickBot="1">
       <c r="A57" s="30"/>
-      <c r="B57" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C57" s="30">
-        <v>11</v>
-      </c>
+      <c r="B57" s="30"/>
+      <c r="C57" s="30"/>
       <c r="D57" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F57" s="30"/>
       <c r="G57" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H57" s="29">
         <v>2</v>
@@ -2300,19 +2070,15 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" s="28">
-        <v>12</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
       <c r="D58" s="28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E58" s="28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F58" s="28"/>
       <c r="G58" s="8" t="s">
@@ -2324,21 +2090,17 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="29"/>
-      <c r="B59" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C59" s="29">
-        <v>12</v>
-      </c>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
       <c r="D59" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F59" s="29"/>
       <c r="G59" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H59" s="29">
         <v>2</v>
@@ -2346,21 +2108,17 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="29"/>
-      <c r="B60" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="29">
-        <v>12</v>
-      </c>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
       <c r="D60" s="29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F60" s="29"/>
       <c r="G60" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H60" s="29">
         <v>2</v>
@@ -2368,21 +2126,17 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="29"/>
-      <c r="B61" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C61" s="29">
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D61" s="29" t="s">
-        <v>13</v>
-      </c>
       <c r="E61" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F61" s="29"/>
       <c r="G61" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H61" s="29">
         <v>2</v>
@@ -2390,21 +2144,17 @@
     </row>
     <row r="62" spans="1:8" ht="16" thickBot="1">
       <c r="A62" s="30"/>
-      <c r="B62" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C62" s="30">
+      <c r="B62" s="30"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D62" s="30" t="s">
-        <v>13</v>
-      </c>
       <c r="E62" s="30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F62" s="30"/>
       <c r="G62" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H62" s="29">
         <v>2</v>
@@ -2412,19 +2162,15 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="B63" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C63" s="28">
-        <v>13</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
       <c r="D63" s="28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F63" s="28"/>
       <c r="G63" s="8" t="s">
@@ -2436,21 +2182,17 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="29"/>
-      <c r="B64" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C64" s="29">
-        <v>13</v>
-      </c>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
       <c r="D64" s="29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F64" s="29"/>
       <c r="G64" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H64" s="29">
         <v>2</v>
@@ -2458,21 +2200,17 @@
     </row>
     <row r="65" spans="1:8" ht="16" thickBot="1">
       <c r="A65" s="30"/>
-      <c r="B65" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C65" s="30">
-        <v>13</v>
-      </c>
+      <c r="B65" s="30"/>
+      <c r="C65" s="30"/>
       <c r="D65" s="30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F65" s="30"/>
       <c r="G65" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H65" s="30">
         <v>2</v>
@@ -2480,23 +2218,19 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="B66" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C66" s="31">
-        <v>16</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B66" s="31"/>
+      <c r="C66" s="31"/>
       <c r="D66" s="31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E66" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F66" s="31"/>
       <c r="G66" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H66" s="33">
         <v>3</v>
@@ -2504,17 +2238,13 @@
     </row>
     <row r="67" spans="1:8" ht="16" thickBot="1">
       <c r="A67" s="32"/>
-      <c r="B67" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C67" s="32">
-        <v>16</v>
-      </c>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
       <c r="D67" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E67" s="32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F67" s="32"/>
       <c r="G67" s="12" t="s">
@@ -2526,19 +2256,15 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="B68" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C68" s="31">
-        <v>17</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B68" s="31"/>
+      <c r="C68" s="31"/>
       <c r="D68" s="31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E68" s="31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F68" s="31"/>
       <c r="G68" s="11" t="s">
@@ -2550,21 +2276,17 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="33"/>
-      <c r="B69" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C69" s="33">
-        <v>17</v>
-      </c>
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
       <c r="D69" s="33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E69" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F69" s="33"/>
       <c r="G69" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H69" s="33">
         <v>3</v>
@@ -2572,21 +2294,17 @@
     </row>
     <row r="70" spans="1:8" ht="16" thickBot="1">
       <c r="A70" s="32"/>
-      <c r="B70" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C70" s="32">
-        <v>17</v>
-      </c>
+      <c r="B70" s="32"/>
+      <c r="C70" s="32"/>
       <c r="D70" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E70" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F70" s="32"/>
       <c r="G70" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H70" s="33">
         <v>3</v>
@@ -2594,23 +2312,19 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="B71" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C71" s="31">
-        <v>18</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B71" s="31"/>
+      <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E71" s="31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F71" s="31"/>
       <c r="G71" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H71" s="33">
         <v>3</v>
@@ -2618,17 +2332,13 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="33"/>
-      <c r="B72" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C72" s="33">
-        <v>18</v>
-      </c>
+      <c r="B72" s="33"/>
+      <c r="C72" s="33"/>
       <c r="D72" s="33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E72" s="33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F72" s="33"/>
       <c r="G72" s="13" t="s">
@@ -2640,21 +2350,17 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="33"/>
-      <c r="B73" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C73" s="33">
-        <v>18</v>
-      </c>
+      <c r="B73" s="33"/>
+      <c r="C73" s="33"/>
       <c r="D73" s="33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E73" s="33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F73" s="33"/>
       <c r="G73" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H73" s="33">
         <v>3</v>
@@ -2662,21 +2368,17 @@
     </row>
     <row r="74" spans="1:8" ht="16" thickBot="1">
       <c r="A74" s="32"/>
-      <c r="B74" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" s="32">
-        <v>18</v>
-      </c>
+      <c r="B74" s="32"/>
+      <c r="C74" s="32"/>
       <c r="D74" s="32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E74" s="32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F74" s="32"/>
       <c r="G74" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H74" s="33">
         <v>3</v>
@@ -2684,19 +2386,15 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="B75" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C75" s="31">
-        <v>19</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B75" s="31"/>
+      <c r="C75" s="31"/>
       <c r="D75" s="31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E75" s="31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F75" s="31"/>
       <c r="G75" s="11" t="s">
@@ -2708,21 +2406,17 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="33"/>
-      <c r="B76" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C76" s="33">
-        <v>19</v>
-      </c>
+      <c r="B76" s="33"/>
+      <c r="C76" s="33"/>
       <c r="D76" s="33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E76" s="33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F76" s="33"/>
       <c r="G76" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H76" s="33">
         <v>3</v>
@@ -2730,21 +2424,17 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="33"/>
-      <c r="B77" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C77" s="33">
-        <v>19</v>
-      </c>
+      <c r="B77" s="33"/>
+      <c r="C77" s="33"/>
       <c r="D77" s="33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E77" s="33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F77" s="33"/>
       <c r="G77" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H77" s="33">
         <v>3</v>
@@ -2752,21 +2442,17 @@
     </row>
     <row r="78" spans="1:8" ht="16" thickBot="1">
       <c r="A78" s="32"/>
-      <c r="B78" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C78" s="32">
-        <v>19</v>
-      </c>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
       <c r="D78" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E78" s="32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F78" s="32"/>
       <c r="G78" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H78" s="33">
         <v>3</v>
@@ -2774,19 +2460,15 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="B79" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C79" s="31">
-        <v>20</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B79" s="31"/>
+      <c r="C79" s="31"/>
       <c r="D79" s="31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E79" s="31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F79" s="31"/>
       <c r="G79" s="11" t="s">
@@ -2798,21 +2480,17 @@
     </row>
     <row r="80" spans="1:8" ht="16" thickBot="1">
       <c r="A80" s="32"/>
-      <c r="B80" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C80" s="32">
-        <v>20</v>
-      </c>
+      <c r="B80" s="32"/>
+      <c r="C80" s="32"/>
       <c r="D80" s="32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E80" s="32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F80" s="32"/>
       <c r="G80" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H80" s="32">
         <v>3</v>
@@ -2820,19 +2498,15 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="B81" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C81" s="34">
-        <v>23</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B81" s="34"/>
+      <c r="C81" s="34"/>
       <c r="D81" s="34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E81" s="34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F81" s="34"/>
       <c r="G81" s="14" t="s">
@@ -2844,21 +2518,17 @@
     </row>
     <row r="82" spans="1:8" ht="16" thickBot="1">
       <c r="A82" s="35"/>
-      <c r="B82" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C82" s="35">
-        <v>23</v>
-      </c>
+      <c r="B82" s="35"/>
+      <c r="C82" s="35"/>
       <c r="D82" s="35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E82" s="35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F82" s="35"/>
       <c r="G82" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H82" s="36">
         <v>4</v>
@@ -2866,23 +2536,19 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="B83" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C83" s="34">
-        <v>24</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B83" s="34"/>
+      <c r="C83" s="34"/>
       <c r="D83" s="34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E83" s="34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F83" s="34"/>
       <c r="G83" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H83" s="36">
         <v>4</v>
@@ -2890,21 +2556,17 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="36"/>
-      <c r="B84" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C84" s="36">
-        <v>24</v>
-      </c>
+      <c r="B84" s="36"/>
+      <c r="C84" s="36"/>
       <c r="D84" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E84" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F84" s="36"/>
       <c r="G84" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H84" s="36">
         <v>4</v>
@@ -2912,21 +2574,17 @@
     </row>
     <row r="85" spans="1:8" ht="16" thickBot="1">
       <c r="A85" s="35"/>
-      <c r="B85" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C85" s="35">
-        <v>24</v>
-      </c>
+      <c r="B85" s="35"/>
+      <c r="C85" s="35"/>
       <c r="D85" s="35" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E85" s="35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F85" s="35"/>
       <c r="G85" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H85" s="36">
         <v>4</v>
@@ -2934,23 +2592,19 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="B86" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C86" s="34">
-        <v>25</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B86" s="34"/>
+      <c r="C86" s="34"/>
       <c r="D86" s="34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E86" s="34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F86" s="34"/>
       <c r="G86" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H86" s="36">
         <v>4</v>
@@ -2958,21 +2612,17 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87" s="36"/>
-      <c r="B87" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C87" s="36">
-        <v>25</v>
-      </c>
+      <c r="B87" s="36"/>
+      <c r="C87" s="36"/>
       <c r="D87" s="36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E87" s="36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F87" s="36"/>
       <c r="G87" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H87" s="36">
         <v>4</v>
@@ -2980,21 +2630,17 @@
     </row>
     <row r="88" spans="1:8" ht="16" thickBot="1">
       <c r="A88" s="35"/>
-      <c r="B88" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C88" s="35">
-        <v>25</v>
-      </c>
+      <c r="B88" s="35"/>
+      <c r="C88" s="35"/>
       <c r="D88" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E88" s="35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F88" s="35"/>
       <c r="G88" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H88" s="36">
         <v>4</v>
@@ -3002,23 +2648,19 @@
     </row>
     <row r="89" spans="1:8">
       <c r="A89" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="B89" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C89" s="34">
-        <v>26</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B89" s="34"/>
+      <c r="C89" s="34"/>
       <c r="D89" s="34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E89" s="34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F89" s="34"/>
       <c r="G89" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H89" s="36">
         <v>4</v>
@@ -3026,21 +2668,17 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90" s="36"/>
-      <c r="B90" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C90" s="36">
-        <v>26</v>
-      </c>
+      <c r="B90" s="36"/>
+      <c r="C90" s="36"/>
       <c r="D90" s="36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E90" s="36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F90" s="36"/>
       <c r="G90" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H90" s="36">
         <v>4</v>
@@ -3048,21 +2686,17 @@
     </row>
     <row r="91" spans="1:8" ht="16" thickBot="1">
       <c r="A91" s="35"/>
-      <c r="B91" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C91" s="35">
-        <v>26</v>
-      </c>
+      <c r="B91" s="35"/>
+      <c r="C91" s="35"/>
       <c r="D91" s="35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E91" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F91" s="35"/>
       <c r="G91" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H91" s="36">
         <v>4</v>
@@ -3070,19 +2704,15 @@
     </row>
     <row r="92" spans="1:8">
       <c r="A92" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="B92" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C92" s="34">
-        <v>27</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B92" s="34"/>
+      <c r="C92" s="34"/>
       <c r="D92" s="34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E92" s="34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F92" s="34"/>
       <c r="G92" s="14" t="s">
@@ -3094,21 +2724,17 @@
     </row>
     <row r="93" spans="1:8" ht="16" thickBot="1">
       <c r="A93" s="35"/>
-      <c r="B93" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C93" s="35">
-        <v>27</v>
-      </c>
+      <c r="B93" s="35"/>
+      <c r="C93" s="35"/>
       <c r="D93" s="35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E93" s="35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F93" s="35"/>
       <c r="G93" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H93" s="35">
         <v>4</v>
@@ -3116,23 +2742,19 @@
     </row>
     <row r="94" spans="1:8">
       <c r="A94" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="B94" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C94" s="37">
-        <v>30</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B94" s="37"/>
+      <c r="C94" s="37"/>
       <c r="D94" s="37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E94" s="37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F94" s="37"/>
       <c r="G94" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H94" s="38">
         <v>5</v>
@@ -3140,21 +2762,17 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95" s="38"/>
-      <c r="B95" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C95" s="38">
-        <v>30</v>
-      </c>
+      <c r="B95" s="38"/>
+      <c r="C95" s="38"/>
       <c r="D95" s="38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E95" s="38" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F95" s="38"/>
       <c r="G95" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H95" s="38">
         <v>5</v>
@@ -3162,17 +2780,13 @@
     </row>
     <row r="96" spans="1:8" ht="16" thickBot="1">
       <c r="A96" s="39"/>
-      <c r="B96" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C96" s="39">
-        <v>30</v>
-      </c>
+      <c r="B96" s="39"/>
+      <c r="C96" s="39"/>
       <c r="D96" s="39" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E96" s="39" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F96" s="39"/>
       <c r="G96" s="19" t="s">
@@ -3184,23 +2798,19 @@
     </row>
     <row r="97" spans="1:8">
       <c r="A97" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="B97" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C97" s="37">
-        <v>1</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B97" s="37"/>
+      <c r="C97" s="37"/>
       <c r="D97" s="37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E97" s="37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F97" s="37"/>
       <c r="G97" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H97" s="38">
         <v>5</v>
@@ -3208,21 +2818,17 @@
     </row>
     <row r="98" spans="1:8">
       <c r="A98" s="38"/>
-      <c r="B98" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C98" s="38">
-        <v>1</v>
-      </c>
+      <c r="B98" s="38"/>
+      <c r="C98" s="38"/>
       <c r="D98" s="38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E98" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F98" s="38"/>
       <c r="G98" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H98" s="38">
         <v>5</v>
@@ -3230,21 +2836,17 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99" s="38"/>
-      <c r="B99" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C99" s="38">
-        <v>1</v>
-      </c>
+      <c r="B99" s="38"/>
+      <c r="C99" s="38"/>
       <c r="D99" s="38" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E99" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F99" s="38"/>
       <c r="G99" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H99" s="38">
         <v>5</v>
@@ -3252,21 +2854,17 @@
     </row>
     <row r="100" spans="1:8" ht="16" thickBot="1">
       <c r="A100" s="39"/>
-      <c r="B100" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C100" s="39">
-        <v>1</v>
-      </c>
+      <c r="B100" s="39"/>
+      <c r="C100" s="39"/>
       <c r="D100" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E100" s="39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F100" s="39"/>
       <c r="G100" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H100" s="38">
         <v>5</v>
@@ -3274,19 +2872,15 @@
     </row>
     <row r="101" spans="1:8">
       <c r="A101" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="B101" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C101" s="37">
-        <v>3</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B101" s="37"/>
+      <c r="C101" s="37"/>
       <c r="D101" s="37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E101" s="37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F101" s="37"/>
       <c r="G101" s="17" t="s">
@@ -3298,21 +2892,17 @@
     </row>
     <row r="102" spans="1:8" ht="16" thickBot="1">
       <c r="A102" s="39"/>
-      <c r="B102" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C102" s="39">
-        <v>3</v>
-      </c>
+      <c r="B102" s="39"/>
+      <c r="C102" s="39"/>
       <c r="D102" s="39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E102" s="39" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F102" s="39"/>
       <c r="G102" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H102" s="38">
         <v>5</v>
@@ -3320,19 +2910,15 @@
     </row>
     <row r="103" spans="1:8">
       <c r="A103" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="B103" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C103" s="37">
-        <v>4</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B103" s="37"/>
+      <c r="C103" s="37"/>
       <c r="D103" s="37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E103" s="37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F103" s="37"/>
       <c r="G103" s="17" t="s">
@@ -3344,21 +2930,17 @@
     </row>
     <row r="104" spans="1:8">
       <c r="A104" s="38"/>
-      <c r="B104" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C104" s="38">
-        <v>4</v>
-      </c>
+      <c r="B104" s="38"/>
+      <c r="C104" s="38"/>
       <c r="D104" s="38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E104" s="38" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F104" s="38"/>
       <c r="G104" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H104" s="38">
         <v>5</v>
@@ -3366,21 +2948,17 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105" s="38"/>
-      <c r="B105" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C105" s="38">
-        <v>4</v>
-      </c>
+      <c r="B105" s="38"/>
+      <c r="C105" s="38"/>
       <c r="D105" s="38" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E105" s="38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F105" s="38"/>
       <c r="G105" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H105" s="38">
         <v>5</v>
@@ -3388,30 +2966,25 @@
     </row>
     <row r="106" spans="1:8" ht="16" thickBot="1">
       <c r="A106" s="39"/>
-      <c r="B106" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C106" s="39">
-        <v>4</v>
-      </c>
+      <c r="B106" s="39"/>
+      <c r="C106" s="39"/>
       <c r="D106" s="39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E106" s="39" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F106" s="39"/>
       <c r="G106" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H106" s="40">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H1:H106"/>
+  <autoFilter ref="G1:H106"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>